<commit_message>
Resources Uses Gantt Chart
Resources Uses Gantt Chart
</commit_message>
<xml_diff>
--- a/Civilworks cost/Spec for EMB PROT Works/Resources.xlsx
+++ b/Civilworks cost/Spec for EMB PROT Works/Resources.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
@@ -765,7 +765,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -776,18 +776,18 @@
   <dimension ref="A1:C14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F11" sqref="F10:F11"/>
+      <selection activeCell="F22" sqref="F22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.5546875" customWidth="1"/>
-    <col min="2" max="2" width="18.33203125" customWidth="1"/>
-    <col min="3" max="3" width="14.33203125" customWidth="1"/>
-    <col min="4" max="4" width="12.6640625" customWidth="1"/>
+    <col min="1" max="1" width="9.5703125" customWidth="1"/>
+    <col min="2" max="2" width="18.28515625" customWidth="1"/>
+    <col min="3" max="3" width="14.28515625" customWidth="1"/>
+    <col min="4" max="4" width="12.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -798,7 +798,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>101</v>
       </c>
@@ -809,7 +809,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>102</v>
       </c>
@@ -820,7 +820,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>103</v>
       </c>
@@ -831,7 +831,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>104</v>
       </c>
@@ -842,7 +842,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>201</v>
       </c>
@@ -853,7 +853,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>202</v>
       </c>
@@ -864,7 +864,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>203</v>
       </c>
@@ -875,7 +875,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>204</v>
       </c>
@@ -886,7 +886,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>205</v>
       </c>
@@ -897,7 +897,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>206</v>
       </c>
@@ -908,7 +908,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>207</v>
       </c>
@@ -919,7 +919,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>301</v>
       </c>
@@ -930,7 +930,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>401</v>
       </c>
@@ -951,17 +951,17 @@
   <dimension ref="A1:Q11"/>
   <sheetViews>
     <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="32.109375" customWidth="1"/>
-    <col min="5" max="5" width="8.88671875" style="1"/>
-    <col min="6" max="6" width="11.21875" customWidth="1"/>
+    <col min="1" max="1" width="32.140625" customWidth="1"/>
+    <col min="5" max="5" width="8.85546875" style="1"/>
+    <col min="6" max="6" width="11.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>1</v>
       </c>
@@ -1014,7 +1014,7 @@
         <v>401</v>
       </c>
     </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
         <v>16</v>
       </c>
@@ -1068,7 +1068,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
         <v>17</v>
       </c>
@@ -1091,7 +1091,7 @@
         <v>0</v>
       </c>
       <c r="H3" s="5">
-        <v>0</v>
+        <v>2500</v>
       </c>
       <c r="I3" s="5">
         <v>350</v>
@@ -1122,7 +1122,7 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
         <v>18</v>
       </c>
@@ -1145,7 +1145,7 @@
         <v>0</v>
       </c>
       <c r="H4" s="5">
-        <v>0</v>
+        <v>500</v>
       </c>
       <c r="I4" s="5">
         <v>90</v>
@@ -1176,7 +1176,7 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
         <v>19</v>
       </c>
@@ -1230,7 +1230,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
         <v>20</v>
       </c>
@@ -1284,7 +1284,7 @@
         <v>7.4999999999999997E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
         <v>21</v>
       </c>
@@ -1338,7 +1338,7 @@
         <v>7.4999999999999997E-2</v>
       </c>
     </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
         <v>22</v>
       </c>
@@ -1392,7 +1392,7 @@
         <v>7.4999999999999997E-2</v>
       </c>
     </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
         <v>23</v>
       </c>
@@ -1446,7 +1446,7 @@
         <v>0.375</v>
       </c>
     </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="s">
         <v>24</v>
       </c>
@@ -1500,7 +1500,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A11" s="3"/>
       <c r="B11" s="3"/>
       <c r="C11" s="3"/>
@@ -1531,13 +1531,13 @@
       <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="26.21875" customWidth="1"/>
+    <col min="2" max="2" width="26.28515625" customWidth="1"/>
     <col min="3" max="95" width="4" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:95" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:95" x14ac:dyDescent="0.25">
       <c r="B2" s="2" t="s">
         <v>34</v>
       </c>
@@ -1821,7 +1821,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="3" spans="2:95" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:95" x14ac:dyDescent="0.25">
       <c r="B3" s="2" t="s">
         <v>3</v>
       </c>
@@ -1919,7 +1919,7 @@
       <c r="CP3" s="7"/>
       <c r="CQ3" s="7"/>
     </row>
-    <row r="4" spans="2:95" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:95" x14ac:dyDescent="0.25">
       <c r="B4" s="2" t="s">
         <v>4</v>
       </c>
@@ -2017,7 +2017,7 @@
       <c r="CP4" s="7"/>
       <c r="CQ4" s="7"/>
     </row>
-    <row r="5" spans="2:95" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:95" x14ac:dyDescent="0.25">
       <c r="B5" s="2" t="s">
         <v>6</v>
       </c>
@@ -2115,7 +2115,7 @@
       <c r="CP5" s="7"/>
       <c r="CQ5" s="7"/>
     </row>
-    <row r="6" spans="2:95" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:95" x14ac:dyDescent="0.25">
       <c r="B6" s="2" t="s">
         <v>7</v>
       </c>
@@ -2213,7 +2213,7 @@
       <c r="CP6" s="7"/>
       <c r="CQ6" s="7"/>
     </row>
-    <row r="7" spans="2:95" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:95" x14ac:dyDescent="0.25">
       <c r="B7" s="2" t="s">
         <v>8</v>
       </c>
@@ -2311,7 +2311,7 @@
       <c r="CP7" s="7"/>
       <c r="CQ7" s="7"/>
     </row>
-    <row r="8" spans="2:95" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:95" x14ac:dyDescent="0.25">
       <c r="B8" s="2" t="s">
         <v>10</v>
       </c>
@@ -2409,7 +2409,7 @@
       <c r="CP8" s="7"/>
       <c r="CQ8" s="7"/>
     </row>
-    <row r="9" spans="2:95" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:95" x14ac:dyDescent="0.25">
       <c r="B9" s="2" t="s">
         <v>29</v>
       </c>
@@ -2507,7 +2507,7 @@
       <c r="CP9" s="7"/>
       <c r="CQ9" s="7"/>
     </row>
-    <row r="10" spans="2:95" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:95" x14ac:dyDescent="0.25">
       <c r="B10" s="2" t="s">
         <v>12</v>
       </c>
@@ -2605,7 +2605,7 @@
       <c r="CP10" s="7"/>
       <c r="CQ10" s="7"/>
     </row>
-    <row r="11" spans="2:95" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:95" x14ac:dyDescent="0.25">
       <c r="B11" s="2" t="s">
         <v>30</v>
       </c>
@@ -2703,7 +2703,7 @@
       <c r="CP11" s="7"/>
       <c r="CQ11" s="7"/>
     </row>
-    <row r="12" spans="2:95" x14ac:dyDescent="0.3">
+    <row r="12" spans="2:95" x14ac:dyDescent="0.25">
       <c r="B12" s="2" t="s">
         <v>31</v>
       </c>
@@ -2801,7 +2801,7 @@
       <c r="CP12" s="7"/>
       <c r="CQ12" s="7"/>
     </row>
-    <row r="13" spans="2:95" x14ac:dyDescent="0.3">
+    <row r="13" spans="2:95" x14ac:dyDescent="0.25">
       <c r="B13" s="2" t="s">
         <v>9</v>
       </c>
@@ -2899,7 +2899,7 @@
       <c r="CP13" s="7"/>
       <c r="CQ13" s="7"/>
     </row>
-    <row r="14" spans="2:95" x14ac:dyDescent="0.3">
+    <row r="14" spans="2:95" x14ac:dyDescent="0.25">
       <c r="B14" s="2" t="s">
         <v>14</v>
       </c>
@@ -2997,7 +2997,7 @@
       <c r="CP14" s="7"/>
       <c r="CQ14" s="7"/>
     </row>
-    <row r="15" spans="2:95" x14ac:dyDescent="0.3">
+    <row r="15" spans="2:95" x14ac:dyDescent="0.25">
       <c r="B15" s="2" t="s">
         <v>32</v>
       </c>

</xml_diff>